<commit_message>
use local v to calc centrifugal
</commit_message>
<xml_diff>
--- a/Calibration/output/20150716 遠心加速度、接線加速度/01 角加速度、差分では不安定？/temp.xlsx
+++ b/Calibration/output/20150716 遠心加速度、接線加速度/01 角加速度、差分では不安定？/temp.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\慶太\Dropbox\Keita Nagara\研究\00.プログラム\python\Spyder\SLAMwithCameraIMUforPython\Calibration\output\20150716 遠心加速度、接線加速度\01 角加速度、差分では不安定？\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="17556" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="temp.csv" sheetId="1" r:id="rId1"/>
@@ -66,6 +71,20 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC0000"/>
+      <color rgb="FF0033CC"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -92,6 +111,13 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="0033CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -102,70 +128,70 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="243"/>
                 <c:pt idx="0">
-                  <c:v>-0.00682831199999999</c:v>
+                  <c:v>-6.82831199999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.008681782</c:v>
+                  <c:v>8.6817820000000007E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0238542877</c:v>
+                  <c:v>2.3854287700000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0432216279999999</c:v>
+                  <c:v>4.3221627999999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.048305183</c:v>
+                  <c:v>4.8305183000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.040851612</c:v>
+                  <c:v>4.0851612000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0371487429999999</c:v>
+                  <c:v>3.7148742999999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.035901438</c:v>
+                  <c:v>3.5901438000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.035348002</c:v>
+                  <c:v>3.5348002000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0350730589999999</c:v>
+                  <c:v>3.50730589999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0349804459999999</c:v>
+                  <c:v>3.4980445999999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.03493935</c:v>
+                  <c:v>3.4939350000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0252119449999999</c:v>
+                  <c:v>2.5211944999999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.001317505</c:v>
+                  <c:v>1.3175050000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.0304118399999999</c:v>
+                  <c:v>-3.0411839999999898E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.0523349869999999</c:v>
+                  <c:v>-5.2334986999999902E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.0523504909999999</c:v>
+                  <c:v>-5.2350490999999902E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.0414855569999999</c:v>
+                  <c:v>-4.1485556999999902E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.0322121169999999</c:v>
+                  <c:v>-3.2212116999999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.013410414</c:v>
+                  <c:v>-1.3410414000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.066826887</c:v>
+                  <c:v>6.6826887000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.112170053</c:v>
+                  <c:v>0.11217005300000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0.134507192999999</c:v>
@@ -174,202 +200,202 @@
                   <c:v>0.212365682999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.243155483</c:v>
+                  <c:v>0.24315548300000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.259611132999999</c:v>
+                  <c:v>0.25961113299999899</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.272956042999999</c:v>
+                  <c:v>0.27295604299999898</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.247818153</c:v>
+                  <c:v>0.24781815300000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.088438713</c:v>
+                  <c:v>8.8438713000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.0818595869999999</c:v>
+                  <c:v>-8.18595869999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-0.204805967</c:v>
+                  <c:v>-0.20480596700000001</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>-0.239597057</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-0.219060197</c:v>
+                  <c:v>-0.21906019700000001</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-0.207040446999999</c:v>
+                  <c:v>-0.20704044699999899</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-0.221844616999999</c:v>
+                  <c:v>-0.22184461699999899</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.226173117</c:v>
+                  <c:v>-0.22617311700000001</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-0.212021007</c:v>
+                  <c:v>-0.21202100700000001</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.179229016999999</c:v>
+                  <c:v>-0.17922901699999899</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>-0.135184526999999</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-0.073887982</c:v>
+                  <c:v>-7.3887982000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-0.049608402</c:v>
+                  <c:v>-4.9608402000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-0.048164651</c:v>
+                  <c:v>-4.8164651000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-0.058841007</c:v>
+                  <c:v>-5.8841007000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-0.085093372</c:v>
+                  <c:v>-8.5093372E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-0.072553747</c:v>
+                  <c:v>-7.2553747000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-0.014814492</c:v>
+                  <c:v>-1.4814492E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.0203063497</c:v>
+                  <c:v>2.03063497E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.080527283</c:v>
+                  <c:v>8.0527283000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>0.116021766999999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.141594663</c:v>
+                  <c:v>0.14159466300000001</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.152115492999999</c:v>
+                  <c:v>0.15211549299999899</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.148753453</c:v>
+                  <c:v>0.14875345300000001</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.129882773</c:v>
+                  <c:v>0.12988277300000001</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>0.110393722999999</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.082500103</c:v>
+                  <c:v>8.2500103000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.0403720639999999</c:v>
+                  <c:v>4.0372063999999902E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.0276224699999999</c:v>
+                  <c:v>2.7622469999999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.007527441</c:v>
+                  <c:v>7.5274410000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-0.016078383</c:v>
+                  <c:v>-1.6078383000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-0.0361481049999999</c:v>
+                  <c:v>-3.6148104999999903E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-0.0365364469999999</c:v>
+                  <c:v>-3.6536446999999903E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-0.027287207</c:v>
+                  <c:v>-2.7287207000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>-0.0138710399999999</c:v>
+                  <c:v>-1.3871039999999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>-0.000388174999999999</c:v>
+                  <c:v>-3.8817499999999901E-4</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.0107243847</c:v>
+                  <c:v>1.0724384700000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.0149154817999999</c:v>
+                  <c:v>1.4915481799999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.0166397219999999</c:v>
+                  <c:v>1.6639721999999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.0170923015599999</c:v>
+                  <c:v>1.7092301559999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.012449826</c:v>
+                  <c:v>1.2449826000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.00552404899999999</c:v>
+                  <c:v>5.5240489999999901E-3</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>-0.0027599</c:v>
+                  <c:v>-2.7599E-3</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>-0.010933761</c:v>
+                  <c:v>-1.0933761E-2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.000350793</c:v>
+                  <c:v>3.5079300000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.011003086</c:v>
+                  <c:v>1.1003086E-2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.0150205941999999</c:v>
+                  <c:v>1.50205941999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.0165357954999999</c:v>
+                  <c:v>1.6535795499999902E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.00733701499999999</c:v>
+                  <c:v>7.3370149999999901E-3</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-0.007000707</c:v>
+                  <c:v>-7.0007070000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>-0.0243818969999999</c:v>
+                  <c:v>-2.4381896999999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>-0.028319217</c:v>
+                  <c:v>-2.8319217000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>-0.00522258699999999</c:v>
+                  <c:v>-5.2225869999999903E-3</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.0238358387</c:v>
+                  <c:v>2.38358387E-2</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.0550738829999999</c:v>
+                  <c:v>5.50738829999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.0690975429999999</c:v>
+                  <c:v>6.90975429999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.081441913</c:v>
+                  <c:v>8.1441913000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>0.101513693</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.122715547999999</c:v>
+                  <c:v>0.12271554799999899</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.128405152999999</c:v>
+                  <c:v>0.12840515299999899</c:v>
                 </c:pt>
                 <c:pt idx="88">
                   <c:v>0.120094983</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.110518522999999</c:v>
+                  <c:v>0.11051852299999899</c:v>
                 </c:pt>
                 <c:pt idx="90">
                   <c:v>0.107292703</c:v>
@@ -387,94 +413,94 @@
                   <c:v>0.120929182999999</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.124239123</c:v>
+                  <c:v>0.12423912300000001</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.147879402999999</c:v>
+                  <c:v>0.14787940299999899</c:v>
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>0.175892453</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.233722003</c:v>
+                  <c:v>0.23372200300000001</c:v>
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>0.272951582999999</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.313695133</c:v>
+                  <c:v>0.31369513300000001</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>0.335725722999999</c:v>
+                  <c:v>0.33572572299999898</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>0.351524113</c:v>
+                  <c:v>0.35152411300000003</c:v>
                 </c:pt>
                 <c:pt idx="103">
                   <c:v>0.370775732999999</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>0.378116962999999</c:v>
+                  <c:v>0.37811696299999897</c:v>
                 </c:pt>
                 <c:pt idx="105">
                   <c:v>0.391116823</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>0.416269983</c:v>
+                  <c:v>0.41626998300000001</c:v>
                 </c:pt>
                 <c:pt idx="107">
                   <c:v>0.458444083</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>0.475270882999999</c:v>
+                  <c:v>0.47527088299999898</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>0.486248312999999</c:v>
+                  <c:v>0.48624831299999899</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>0.498641282999999</c:v>
+                  <c:v>0.49864128299999899</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>0.532283083</c:v>
+                  <c:v>0.53228308300000005</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>0.551233583</c:v>
+                  <c:v>0.55123358300000003</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>0.566633552999999</c:v>
+                  <c:v>0.56663355299999896</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>0.584827383</c:v>
+                  <c:v>0.58482738300000003</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>0.601620523</c:v>
+                  <c:v>0.60162052300000002</c:v>
                 </c:pt>
                 <c:pt idx="116">
                   <c:v>0.681668582999999</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>0.716980083</c:v>
+                  <c:v>0.71698008300000005</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>0.742696012999999</c:v>
+                  <c:v>0.74269601299999899</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>0.768131342999999</c:v>
+                  <c:v>0.76813134299999897</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>0.788595182999999</c:v>
+                  <c:v>0.78859518299999898</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>0.800092683</c:v>
+                  <c:v>0.80009268300000003</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>0.834208983</c:v>
+                  <c:v>0.83420898300000002</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>0.913272882999999</c:v>
+                  <c:v>0.91327288299999898</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>0.953204683</c:v>
+                  <c:v>0.95320468300000005</c:v>
                 </c:pt>
                 <c:pt idx="125">
                   <c:v>0.994636622999999</c:v>
@@ -486,16 +512,16 @@
                   <c:v>1.14009078299999</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>1.17404188299999</c:v>
+                  <c:v>1.1740418829999899</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>1.192873883</c:v>
+                  <c:v>1.1928738830000001</c:v>
                 </c:pt>
                 <c:pt idx="130">
                   <c:v>1.19997658299999</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>1.190398183</c:v>
+                  <c:v>1.1903981830000001</c:v>
                 </c:pt>
                 <c:pt idx="132">
                   <c:v>1.14027708299999</c:v>
@@ -504,13 +530,13 @@
                   <c:v>1.122860983</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>1.14384538299999</c:v>
+                  <c:v>1.1438453829999899</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>1.23072938299999</c:v>
+                  <c:v>1.2307293829999899</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>1.41458458299999</c:v>
+                  <c:v>1.4145845829999899</c:v>
                 </c:pt>
                 <c:pt idx="137">
                   <c:v>1.51861608299999</c:v>
@@ -519,52 +545,52 @@
                   <c:v>1.649027883</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>1.791174583</c:v>
+                  <c:v>1.7911745830000001</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>1.95364748299999</c:v>
+                  <c:v>1.9536474829999899</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>1.90358598299999</c:v>
+                  <c:v>1.9035859829999899</c:v>
                 </c:pt>
                 <c:pt idx="142">
                   <c:v>1.81517928299999</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>1.782700383</c:v>
+                  <c:v>1.7827003830000001</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>1.78862668299999</c:v>
+                  <c:v>1.7886266829999899</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>1.82937118299999</c:v>
+                  <c:v>1.8293711829999899</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>1.800009683</c:v>
+                  <c:v>1.8000096830000001</c:v>
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>1.76595208299999</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>1.730128483</c:v>
+                  <c:v>1.7301284830000001</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>1.711827283</c:v>
+                  <c:v>1.7118272830000001</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>1.73269408299999</c:v>
+                  <c:v>1.7326940829999899</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>1.69273098299999</c:v>
+                  <c:v>1.6927309829999899</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>1.631083483</c:v>
+                  <c:v>1.6310834830000001</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>1.58418088299999</c:v>
+                  <c:v>1.5841808829999899</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>1.53789838299999</c:v>
+                  <c:v>1.5378983829999899</c:v>
                 </c:pt>
                 <c:pt idx="155">
                   <c:v>1.54034608299999</c:v>
@@ -576,259 +602,259 @@
                   <c:v>1.51039668299999</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>1.48835978299999</c:v>
+                  <c:v>1.4883597829999899</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>1.48829088299999</c:v>
+                  <c:v>1.4882908829999899</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>1.55547508299999</c:v>
+                  <c:v>1.5554750829999899</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>1.612543883</c:v>
+                  <c:v>1.6125438830000001</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>1.658947283</c:v>
+                  <c:v>1.6589472830000001</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>1.677873683</c:v>
+                  <c:v>1.6778736830000001</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>1.606313083</c:v>
+                  <c:v>1.6063130830000001</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>1.477806683</c:v>
+                  <c:v>1.4778066830000001</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>1.43244428299999</c:v>
+                  <c:v>1.4324442829999899</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>1.419051883</c:v>
+                  <c:v>1.4190518830000001</c:v>
                 </c:pt>
                 <c:pt idx="168">
                   <c:v>1.401176183</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>1.303658283</c:v>
+                  <c:v>1.3036582830000001</c:v>
                 </c:pt>
                 <c:pt idx="170">
                   <c:v>1.13383288299999</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>0.985164982999999</c:v>
+                  <c:v>0.98516498299999899</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>0.854617383</c:v>
+                  <c:v>0.85461738300000001</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>0.804845883</c:v>
+                  <c:v>0.80484588300000004</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>0.803490883</c:v>
+                  <c:v>0.80349088300000004</c:v>
                 </c:pt>
                 <c:pt idx="175">
                   <c:v>0.792095883</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>0.777053322999999</c:v>
+                  <c:v>0.77705332299999896</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>0.771380033</c:v>
+                  <c:v>0.77138003300000002</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>0.547100683</c:v>
+                  <c:v>0.54710068300000003</c:v>
                 </c:pt>
                 <c:pt idx="179">
                   <c:v>0.387308562999999</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>0.221040693</c:v>
+                  <c:v>0.22104069300000001</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>0.047466923</c:v>
+                  <c:v>4.7466923000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>-0.0203450509999999</c:v>
+                  <c:v>-2.0345050999999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>-0.0126753409999999</c:v>
+                  <c:v>-1.2675340999999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>0.0137942246</c:v>
+                  <c:v>1.37942246E-2</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>-0.0384591599999999</c:v>
+                  <c:v>-3.8459159999999902E-2</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>-0.0629924169999999</c:v>
+                  <c:v>-6.2992416999999898E-2</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>-0.026498957</c:v>
+                  <c:v>-2.6498957E-2</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>0.0249305366999999</c:v>
+                  <c:v>2.4930536699999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>0.027485043</c:v>
+                  <c:v>2.7485043000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>-0.014199041</c:v>
+                  <c:v>-1.4199041000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>-0.0156618619999999</c:v>
+                  <c:v>-1.5661861999999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>0.0881267929999999</c:v>
+                  <c:v>8.8126792999999898E-2</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>0.128456102999999</c:v>
+                  <c:v>0.12845610299999899</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>0.105783679</c:v>
+                  <c:v>0.10578367900000001</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>0.0807614229999999</c:v>
+                  <c:v>8.0761422999999902E-2</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>0.0645676629999999</c:v>
+                  <c:v>6.45676629999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>0.00636684799999999</c:v>
+                  <c:v>6.3668479999999901E-3</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>-0.036011687</c:v>
+                  <c:v>-3.6011687000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>-0.0487224009999999</c:v>
+                  <c:v>-4.8722400999999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>-0.0509880169999999</c:v>
+                  <c:v>-5.0988016999999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>-0.0517511819999999</c:v>
+                  <c:v>-5.1751181999999903E-2</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>-0.0437877509999999</c:v>
+                  <c:v>-4.3787750999999903E-2</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>0.0048233065</c:v>
+                  <c:v>4.8233065E-3</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>0.0291954864999999</c:v>
+                  <c:v>2.9195486499999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>0.010336196</c:v>
+                  <c:v>1.0336196000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>-0.0182537969999999</c:v>
+                  <c:v>-1.8253796999999902E-2</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>-0.052297041</c:v>
+                  <c:v>-5.2297041000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>-0.0534977969999999</c:v>
+                  <c:v>-5.3497796999999903E-2</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>-0.0678663969999999</c:v>
+                  <c:v>-6.7866396999999898E-2</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>-0.0751064669999999</c:v>
+                  <c:v>-7.5106466999999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>-0.055476703</c:v>
+                  <c:v>-5.5476703000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>-0.0343220369999999</c:v>
+                  <c:v>-3.4322036999999903E-2</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>-0.004601985</c:v>
+                  <c:v>-4.6019850000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>0.00167386599999999</c:v>
+                  <c:v>1.67386599999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>-0.00896647199999999</c:v>
+                  <c:v>-8.9664719999999892E-3</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>-0.00590993499999999</c:v>
+                  <c:v>-5.9099349999999903E-3</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>-0.00524026899999999</c:v>
+                  <c:v>-5.2402689999999901E-3</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>-0.0128471609999999</c:v>
+                  <c:v>-1.28471609999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>0.00231304299999999</c:v>
+                  <c:v>2.3130429999999899E-3</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>0.044355519</c:v>
+                  <c:v>4.4355519000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>0.0439876059999999</c:v>
+                  <c:v>4.3987605999999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>0.0168995390999999</c:v>
+                  <c:v>1.6899539099999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>-0.00894554699999999</c:v>
+                  <c:v>-8.9455469999999895E-3</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>-0.0233875399999999</c:v>
+                  <c:v>-2.3387539999999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>-0.023827397</c:v>
+                  <c:v>-2.3827397E-2</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>-0.008986496</c:v>
+                  <c:v>-8.9864960000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>-0.00883065</c:v>
+                  <c:v>-8.8306500000000007E-3</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>-0.0359428529999999</c:v>
+                  <c:v>-3.59428529999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>-0.0278836119999999</c:v>
+                  <c:v>-2.7883611999999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>-0.0281218769999999</c:v>
+                  <c:v>-2.8121876999999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>-0.0323477429999999</c:v>
+                  <c:v>-3.2347742999999901E-2</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>-0.0339415269999999</c:v>
+                  <c:v>-3.3941526999999902E-2</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>-0.034478393</c:v>
+                  <c:v>-3.4478393000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>-0.020520531</c:v>
+                  <c:v>-2.0520531000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>0.00313147399999999</c:v>
+                  <c:v>3.13147399999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>0.0110986195</c:v>
+                  <c:v>1.10986195E-2</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>0.0102133364</c:v>
+                  <c:v>1.02133364E-2</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>0.00385194899999999</c:v>
+                  <c:v>3.8519489999999899E-3</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>0.0020107375</c:v>
+                  <c:v>2.0107375E-3</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>0.00123484099999999</c:v>
+                  <c:v>1.23484099999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>0.000758342999999999</c:v>
+                  <c:v>7.58342999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>0.0672270229999999</c:v>
+                  <c:v>6.72270229999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -838,6 +864,13 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="1"/>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CC0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -848,94 +881,94 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="243"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.344669997321999</c:v>
+                  <c:v>0.34466999732199899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.489433499566</c:v>
+                  <c:v>0.48943349956600002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.496601067934999</c:v>
+                  <c:v>0.49660106793499897</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.163984918712999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.225865840098</c:v>
+                  <c:v>-0.22586584009800001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-0.123429084378</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.0461965663309999</c:v>
+                  <c:v>-4.6196566330999903E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.0197654892971</c:v>
+                  <c:v>-1.9765489297100002E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.0101830927773999</c:v>
+                  <c:v>-1.0183092777399899E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.00330759339883</c:v>
+                  <c:v>-3.30759339883E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.00141711295512999</c:v>
+                  <c:v>-1.41711295512999E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.374130632186</c:v>
+                  <c:v>-0.37413063218600001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.74669973677</c:v>
+                  <c:v>-0.74669973677000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.991540021836999</c:v>
+                  <c:v>-0.99154002183699896</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.685102059758999</c:v>
+                  <c:v>-0.68510205975899896</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.000500126816710999</c:v>
+                  <c:v>-5.00126816710999E-4</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.350482884842999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.264954778820999</c:v>
+                  <c:v>0.26495477882099899</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.522269334082</c:v>
+                  <c:v>0.52226933408200005</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.11151523396</c:v>
+                  <c:v>2.1115152339600001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.22548503463999</c:v>
+                  <c:v>1.2254850346399899</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.638206782361</c:v>
+                  <c:v>0.63820678236100004</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>2.35934872728</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.78948135629</c:v>
+                  <c:v>0.78948135629000005</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.514238020366999</c:v>
+                  <c:v>0.51423802036699895</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.351183058373</c:v>
+                  <c:v>0.35118305837300001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.761754418536999</c:v>
+                  <c:v>-0.76175441853699899</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-4.82964622333</c:v>
+                  <c:v>-4.8296462233300002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-5.16055573854</c:v>
+                  <c:v>-5.1605557385400003</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>-3.72564874013</c:v>
@@ -944,73 +977,73 @@
                   <c:v>-1.15970410597999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.641780356031</c:v>
+                  <c:v>0.64178035603100003</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.387732153325999</c:v>
+                  <c:v>0.38773215332599897</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-0.493472803946</c:v>
+                  <c:v>-0.49347280394600002</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.131166696992</c:v>
+                  <c:v>-0.13116669699200001</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.488003054888999</c:v>
+                  <c:v>0.48800305488899898</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>1.02474761078999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.42079463314</c:v>
+                  <c:v>1.4207946331400001</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.65666602581</c:v>
+                  <c:v>1.6566660258100001</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.837225630059999</c:v>
+                  <c:v>0.83722563005999895</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.048125079229</c:v>
+                  <c:v>4.8125079229000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>-0.355878872725999</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-0.820384743692999</c:v>
+                  <c:v>-0.82038474369299896</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.417987898623999</c:v>
+                  <c:v>0.41798789862399899</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.74967479845</c:v>
+                  <c:v>1.7496747984500001</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.06426817635999</c:v>
+                  <c:v>1.0642681763599899</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.77119567359</c:v>
+                  <c:v>1.7711956735900001</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>1.07559067290999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.799157334647999</c:v>
+                  <c:v>0.79915733464799898</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.276863169153</c:v>
+                  <c:v>0.27686316915300002</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-0.0908660911544</c:v>
+                  <c:v>-9.0866091154400003E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-0.571838920083999</c:v>
+                  <c:v>-0.57183892008399895</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-0.609031578262</c:v>
+                  <c:v>-0.60903157826200005</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-0.84526140754</c:v>
+                  <c:v>-0.84526140754000001</c:v>
                 </c:pt>
                 <c:pt idx="55">
                   <c:v>-1.05320197941</c:v>
@@ -1022,97 +1055,97 @@
                   <c:v>-0.574142277741999</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-0.761480676698999</c:v>
+                  <c:v>-0.76148067669899899</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-0.668991371333</c:v>
+                  <c:v>-0.66899137133300002</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-0.0121356629064</c:v>
+                  <c:v>-1.21356629064E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.289038164247</c:v>
+                  <c:v>0.28903816424700002</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.383320728288999</c:v>
+                  <c:v>0.38332072828899899</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.396553006521</c:v>
+                  <c:v>0.39655300652100001</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.317503089918</c:v>
+                  <c:v>0.31750308991800003</c:v>
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>0.123266987812</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.0522497151101</c:v>
+                  <c:v>5.2249715110100001E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.0150859997204999</c:v>
+                  <c:v>1.50859997204999E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>-0.165803421416999</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>-0.247348150767</c:v>
+                  <c:v>-0.24734815076700001</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>-0.258872881629</c:v>
+                  <c:v>-0.25887288162900002</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>-0.255434541733</c:v>
+                  <c:v>-0.25543454173300001</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.341956260876</c:v>
+                  <c:v>0.34195626087600001</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.295896918037</c:v>
+                  <c:v>0.29589691803700002</c:v>
                 </c:pt>
                 <c:pt idx="74">
                   <c:v>0.125546876821999</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.0473499446676</c:v>
+                  <c:v>4.7349944667600001E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-0.287463449832999</c:v>
+                  <c:v>-0.28746344983299899</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-0.434476524691</c:v>
+                  <c:v>-0.43447652469100001</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>-0.496604210745999</c:v>
+                  <c:v>-0.49660421074599898</c:v>
                 </c:pt>
                 <c:pt idx="79">
                   <c:v>-0.112494581272</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.659906591249999</c:v>
+                  <c:v>0.65990659124999895</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.908073962860999</c:v>
+                  <c:v>0.90807396286099895</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.867723130962</c:v>
+                  <c:v>0.86772313096200004</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.412461560050999</c:v>
+                  <c:v>0.41246156005099899</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.308607704865999</c:v>
+                  <c:v>0.30860770486599898</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.627246527198999</c:v>
+                  <c:v>0.62724652719899898</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.683927776671</c:v>
+                  <c:v>0.68392777667100002</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.183536243664</c:v>
+                  <c:v>0.18353624366400001</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>-0.259692286218999</c:v>
+                  <c:v>-0.25969228621899898</c:v>
                 </c:pt>
                 <c:pt idx="89">
                   <c:v>-0.290195824667</c:v>
@@ -1121,10 +1154,10 @@
                   <c:v>-0.107527435879</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>-0.0534187176107</c:v>
+                  <c:v>-5.3418717610700002E-2</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.206499196933</c:v>
+                  <c:v>0.20649919693300001</c:v>
                 </c:pt>
                 <c:pt idx="93">
                   <c:v>0.149017307178999</c:v>
@@ -1136,28 +1169,28 @@
                   <c:v>0.106772606244999</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.738757252866</c:v>
+                  <c:v>0.73875725286600002</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.903649720951</c:v>
+                  <c:v>0.90364972095100005</c:v>
                 </c:pt>
                 <c:pt idx="98">
                   <c:v>1.52182598556</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.18877542635</c:v>
+                  <c:v>1.1887754263500001</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.19834252934</c:v>
+                  <c:v>1.1983425293400001</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>0.629443884982999</c:v>
+                  <c:v>0.62944388498299897</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>0.405086566473</c:v>
+                  <c:v>0.40508656647300001</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>0.506623333558</c:v>
+                  <c:v>0.50662333355800004</c:v>
                 </c:pt>
                 <c:pt idx="104">
                   <c:v>0.244707900037999</c:v>
@@ -1166,58 +1199,58 @@
                   <c:v>0.448270356373</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>0.838439466264999</c:v>
+                  <c:v>0.83843946626499899</c:v>
                 </c:pt>
                 <c:pt idx="107">
                   <c:v>1.1715023433</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>0.560893868243</c:v>
+                  <c:v>0.56089386824300003</c:v>
                 </c:pt>
                 <c:pt idx="109">
                   <c:v>0.313640088001999</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>0.326129872777999</c:v>
+                  <c:v>0.32612987277799899</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>0.961198476207</c:v>
+                  <c:v>0.96119847620700005</c:v>
                 </c:pt>
                 <c:pt idx="112">
                   <c:v>0.498695966672</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>0.466665865465999</c:v>
+                  <c:v>0.46666586546599897</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>0.491725920937</c:v>
+                  <c:v>0.49172592093700002</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>0.390538295443</c:v>
+                  <c:v>0.39053829544300001</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>2.16346453839999</c:v>
+                  <c:v>2.1634645383999902</c:v>
                 </c:pt>
                 <c:pt idx="117">
                   <c:v>1.03856869365</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>0.779270786222999</c:v>
+                  <c:v>0.77927078622299895</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>0.770767753953999</c:v>
+                  <c:v>0.77076775395399899</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>0.660126023606</c:v>
+                  <c:v>0.66012602360600003</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>0.338160190172999</c:v>
+                  <c:v>0.33816019017299898</c:v>
                 </c:pt>
                 <c:pt idx="122">
                   <c:v>1.06614015777</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>2.39587631148999</c:v>
+                  <c:v>2.3958763114899901</c:v>
                 </c:pt>
                 <c:pt idx="124">
                   <c:v>1.28811687431999</c:v>
@@ -1226,13 +1259,13 @@
                   <c:v>1.33651855187</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>1.88236368528</c:v>
+                  <c:v>1.8823636852800001</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>2.24259724056999</c:v>
+                  <c:v>2.2425972405699901</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>0.943085761345999</c:v>
+                  <c:v>0.94308576134599897</c:v>
                 </c:pt>
                 <c:pt idx="129">
                   <c:v>0.570666798601</c:v>
@@ -1241,40 +1274,40 @@
                   <c:v>0.215233383094</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>-0.342084292823999</c:v>
+                  <c:v>-0.34208429282399899</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>-1.72831117864</c:v>
+                  <c:v>-1.7283111786400001</c:v>
                 </c:pt>
                 <c:pt idx="133">
                   <c:v>-0.600554263939999</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>0.699480667076999</c:v>
+                  <c:v>0.69948066707699896</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>2.55541778561999</c:v>
+                  <c:v>2.5554177856199898</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>4.71423174743</c:v>
+                  <c:v>4.7142317474300004</c:v>
                 </c:pt>
                 <c:pt idx="137">
                   <c:v>3.15247042579999</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>3.95187364092</c:v>
+                  <c:v>3.9518736409200002</c:v>
                 </c:pt>
                 <c:pt idx="139">
                   <c:v>4.44207537287999</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>5.24107838122</c:v>
+                  <c:v>5.2410783812200004</c:v>
                 </c:pt>
                 <c:pt idx="141">
                   <c:v>-1.66871825807999</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>-2.67899152846</c:v>
+                  <c:v>-2.6789915284600001</c:v>
                 </c:pt>
                 <c:pt idx="143">
                   <c:v>-1.01496356811999</c:v>
@@ -1283,22 +1316,22 @@
                   <c:v>0.204354863280999</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>1.10120446247999</c:v>
+                  <c:v>1.1012044624799899</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>-0.793555322194</c:v>
+                  <c:v>-0.79355532219400005</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>-0.973071899445</c:v>
+                  <c:v>-0.97307189944500005</c:v>
                 </c:pt>
                 <c:pt idx="148">
                   <c:v>-0.995099630944</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>-0.538271856477</c:v>
+                  <c:v>-0.53827185647700004</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>0.719543739115</c:v>
+                  <c:v>0.71954373911500003</c:v>
                 </c:pt>
                 <c:pt idx="151">
                   <c:v>-1.14180005709999</c:v>
@@ -1310,79 +1343,79 @@
                   <c:v>-1.56340906611999</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>-1.49298873953</c:v>
+                  <c:v>-1.4929887395300001</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>0.0815900778103999</c:v>
+                  <c:v>8.1590077810399897E-2</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>0.904145663577999</c:v>
+                  <c:v>0.90414566357799897</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>-1.70817295389999</c:v>
+                  <c:v>-1.7081729538999899</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>-0.78703557406</c:v>
+                  <c:v>-0.78703557406000002</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>-0.00229666885693</c:v>
+                  <c:v>-2.29666885693E-3</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>2.23945767143999</c:v>
+                  <c:v>2.2394576714399901</c:v>
                 </c:pt>
                 <c:pt idx="161">
                   <c:v>1.78340967324999</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>1.40616396145999</c:v>
+                  <c:v>1.4061639614599899</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>0.630880601655</c:v>
+                  <c:v>0.63088060165500004</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>-2.04458355749</c:v>
+                  <c:v>-2.0445835574900002</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>-3.67160242468</c:v>
+                  <c:v>-3.6716024246800001</c:v>
                 </c:pt>
                 <c:pt idx="166">
                   <c:v>-1.51208144202999</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>-0.461806197965999</c:v>
+                  <c:v>-0.46180619796599898</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>-0.541688004022999</c:v>
+                  <c:v>-0.54168800402299899</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>-3.25059976668</c:v>
+                  <c:v>-3.2505997666800002</c:v>
                 </c:pt>
                 <c:pt idx="170">
                   <c:v>-6.06521929939999</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>-5.30954579440999</c:v>
+                  <c:v>-5.3095457944099902</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>-4.35159081666999</c:v>
+                  <c:v>-4.3515908166699901</c:v>
                 </c:pt>
                 <c:pt idx="173">
                   <c:v>-1.55535622297999</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>-0.0410606155536</c:v>
+                  <c:v>-4.1060615553600001E-2</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>-0.299869459604</c:v>
+                  <c:v>-0.29986945960400002</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>-0.470079047357999</c:v>
+                  <c:v>-0.47007904735799899</c:v>
                 </c:pt>
                 <c:pt idx="177">
                   <c:v>-0.162093602497</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>-6.40800936527999</c:v>
+                  <c:v>-6.4080093652799901</c:v>
                 </c:pt>
                 <c:pt idx="179">
                   <c:v>-5.15456168156999</c:v>
@@ -1391,19 +1424,19 @@
                   <c:v>-4.49373339741999</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>-5.78579785109999</c:v>
+                  <c:v>-5.7857978510999901</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>-2.05490877811</c:v>
+                  <c:v>-2.0549087781100002</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>0.225580237379999</c:v>
+                  <c:v>0.22558023737999899</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>0.778513010402</c:v>
+                  <c:v>0.77851301040200005</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>-1.41225589468999</c:v>
+                  <c:v>-1.4122558946899899</c:v>
                 </c:pt>
                 <c:pt idx="186">
                   <c:v>-0.791397967807</c:v>
@@ -1412,49 +1445,49 @@
                   <c:v>1.17720317212</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>1.51263573162</c:v>
+                  <c:v>1.5126357316200001</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>0.0824030639890999</c:v>
+                  <c:v>8.2403063989099898E-2</c:v>
                 </c:pt>
                 <c:pt idx="190">
                   <c:v>-1.26315435263999</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>-0.0471879280710999</c:v>
+                  <c:v>-4.7187928071099901E-2</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>3.14511148471</c:v>
+                  <c:v>3.1451114847100001</c:v>
                 </c:pt>
                 <c:pt idx="193">
                   <c:v>1.1522631743</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>-0.708517093013</c:v>
+                  <c:v>-0.70851709301300003</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>-0.807165972665</c:v>
+                  <c:v>-0.80716597266500001</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>-0.462677722515999</c:v>
+                  <c:v>-0.46267772251599898</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>-1.66288767818999</c:v>
+                  <c:v>-1.6628876781899899</c:v>
                 </c:pt>
                 <c:pt idx="198">
                   <c:v>-1.14536764116</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>-0.397209007532999</c:v>
+                  <c:v>-0.39720900753299898</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>-0.0755206053554</c:v>
+                  <c:v>-7.5520605355400006E-2</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>-0.0238488579188999</c:v>
+                  <c:v>-2.3848857918899902E-2</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>0.2413161467</c:v>
+                  <c:v>0.24131614670000001</c:v>
                 </c:pt>
                 <c:pt idx="203">
                   <c:v>1.38888395117999</c:v>
@@ -1463,16 +1496,16 @@
                   <c:v>0.761634756124</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>-0.589351633769999</c:v>
+                  <c:v>-0.58935163376999899</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>-0.714750506638999</c:v>
+                  <c:v>-0.71475050663899897</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>-0.895872323961</c:v>
+                  <c:v>-0.89587232396100003</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>-0.0343074638543999</c:v>
+                  <c:v>-3.4307463854399901E-2</c:v>
                 </c:pt>
                 <c:pt idx="209">
                   <c:v>-0.399127629752</c:v>
@@ -1481,100 +1514,100 @@
                   <c:v>-0.226251728988</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>0.633215388422999</c:v>
+                  <c:v>0.63321538842299896</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>0.682410805952999</c:v>
+                  <c:v>0.68241080595299897</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>0.900607844579</c:v>
+                  <c:v>0.90060784457900001</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>0.17930958885</c:v>
+                  <c:v>0.17930958885000001</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>-0.343237828959</c:v>
+                  <c:v>-0.34323782895900001</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>0.0955165876801</c:v>
+                  <c:v>9.5516587680100004E-2</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>0.0209270200902</c:v>
+                  <c:v>2.0927020090200001E-2</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>-0.253563308483</c:v>
+                  <c:v>-0.25356330848300002</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>0.445889403517</c:v>
+                  <c:v>0.44588940351700002</c:v>
                 </c:pt>
                 <c:pt idx="220">
                   <c:v>1.35621332576999</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>-0.0126866359809999</c:v>
+                  <c:v>-1.2686635980999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>-0.934069859423</c:v>
+                  <c:v>-0.93406985942300003</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>-0.861503691593999</c:v>
+                  <c:v>-0.86150369159399898</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>-0.497999005285</c:v>
+                  <c:v>-0.49799900528500002</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>-0.0125673120382999</c:v>
+                  <c:v>-1.25673120382999E-2</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>0.530034489338</c:v>
+                  <c:v>0.53003448933800001</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>0.0048701776303</c:v>
+                  <c:v>4.8701776303000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>-0.774637748580999</c:v>
+                  <c:v>-0.77463774858099899</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>0.230263463894999</c:v>
+                  <c:v>0.23026346389499899</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>-0.00722015318441</c:v>
+                  <c:v>-7.2201531844100003E-3</c:v>
                 </c:pt>
                 <c:pt idx="231">
                   <c:v>-0.117385123132</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>-0.0514121593424</c:v>
+                  <c:v>-5.1412159342400003E-2</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>-0.0178955503999</c:v>
+                  <c:v>-1.7895550399900002E-2</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>0.465262510376</c:v>
+                  <c:v>0.46526251037600003</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>0.716727589944999</c:v>
+                  <c:v>0.71672758994499897</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>0.257005531630999</c:v>
+                  <c:v>0.25700553163099898</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>-0.0268267668081999</c:v>
+                  <c:v>-2.6826766808199901E-2</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>-0.205205136108</c:v>
+                  <c:v>-0.20520513610800001</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>-0.0613737751973</c:v>
+                  <c:v>-6.1373775197300001E-2</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>-0.0258632413317999</c:v>
+                  <c:v>-2.5863241331799899E-2</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>-0.0140146800793</c:v>
+                  <c:v>-1.40146800793E-2</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>2.21562477965</c:v>
+                  <c:v>2.2156247796500002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1589,13 +1622,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2121319144"/>
-        <c:axId val="-2104884648"/>
+        <c:axId val="328752584"/>
+        <c:axId val="328750232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2121319144"/>
+        <c:axId val="328752584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1604,7 +1636,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104884648"/>
+        <c:crossAx val="328750232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1612,7 +1644,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2104884648"/>
+        <c:axId val="328750232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1623,7 +1655,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121319144"/>
+        <c:crossAx val="328752584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2004,13 +2036,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:II7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
       <selection activeCell="II2" sqref="A2:II7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:243">
+    <row r="1" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -2741,7 +2773,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:243">
+    <row r="2" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>-6.82831199999999E-3</v>
       </c>
@@ -3472,7 +3504,7 @@
         <v>6.72270229999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:243">
+    <row r="3" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1.2113462999999901E-2</v>
       </c>
@@ -4203,7 +4235,7 @@
         <v>3.1046233999999898E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:243">
+    <row r="4" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>-9.7548070000000008E-3</v>
       </c>
@@ -4934,7 +4966,7 @@
         <v>3.6607921000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:243">
+    <row r="5" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -5665,7 +5697,7 @@
         <v>2.2156247796500002</v>
       </c>
     </row>
-    <row r="6" spans="1:243">
+    <row r="6" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -6396,7 +6428,7 @@
         <v>1.3559755931599899</v>
       </c>
     </row>
-    <row r="7" spans="1:243">
+    <row r="7" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0</v>
       </c>

</xml_diff>